<commit_message>
update of the global variables definition 	modified:   globalVariables.xlsx
</commit_message>
<xml_diff>
--- a/globalVariables.xlsx
+++ b/globalVariables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="15140" yWindow="1360" windowWidth="12520" windowHeight="12300" tabRatio="500"/>
+    <workbookView xWindow="11040" yWindow="1360" windowWidth="16620" windowHeight="12300" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -102,21 +102,6 @@
     <t>thread_regulation, thread_ihm</t>
   </si>
   <si>
-    <t>cst_speed_min</t>
-  </si>
-  <si>
-    <t>cst_speed_max</t>
-  </si>
-  <si>
-    <t>cst_inc_dec</t>
-  </si>
-  <si>
-    <t>cst_throttle_sat</t>
-  </si>
-  <si>
-    <t>pedals_min</t>
-  </si>
-  <si>
     <t>uint8</t>
   </si>
   <si>
@@ -130,6 +115,21 @@
   </si>
   <si>
     <t>Glabal variables</t>
+  </si>
+  <si>
+    <t>CST_SPEED_MIN</t>
+  </si>
+  <si>
+    <t>CST_SPEED_MAX</t>
+  </si>
+  <si>
+    <t>CST_INC_DEC</t>
+  </si>
+  <si>
+    <t>CST_THROTTLE_SAT</t>
+  </si>
+  <si>
+    <t>CST_PEDALS_MIN</t>
   </si>
 </sst>
 </file>
@@ -594,7 +594,7 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -606,7 +606,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D1" t="s">
         <v>14</v>
@@ -685,7 +685,7 @@
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D9" t="s">
         <v>17</v>
@@ -699,7 +699,7 @@
         <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D10" t="s">
         <v>16</v>
@@ -713,7 +713,7 @@
         <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D11" t="s">
         <v>16</v>
@@ -780,7 +780,7 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B16" t="s">
         <v>19</v>
@@ -794,7 +794,7 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B17" t="s">
         <v>19</v>
@@ -808,12 +808,12 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B21" t="s">
         <v>10</v>
@@ -821,7 +821,7 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B22" t="s">
         <v>10</v>
@@ -829,7 +829,7 @@
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B23" t="s">
         <v>10</v>
@@ -837,23 +837,22 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B24" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B25" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>